<commit_message>
Added correct columns to requirements_traceability.xlsx in REQM
</commit_message>
<xml_diff>
--- a/Evidence/REQM/requirements_traceability.xlsx
+++ b/Evidence/REQM/requirements_traceability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raygu\Downloads\CO3095-Group-16-Music-Player-Application\Evidence\REQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44EB7A7-0D18-4A50-BC3A-164206701CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E2C706-65C5-49D8-834B-2D2BD68F6082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{69E9F38F-E908-4412-9BBE-056D5BFD6B03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
   <si>
     <t>Story ID</t>
   </si>
@@ -330,6 +330,36 @@
   </si>
   <si>
     <t>S4-12</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Priority (MoSCoW)</t>
+  </si>
+  <si>
+    <t>Must</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria Summary</t>
+  </si>
+  <si>
+    <t>Code Modules / Files</t>
+  </si>
+  <si>
+    <t>Test Cases / Files</t>
+  </si>
+  <si>
+    <t>Coverage %</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Evidence Link (Branch)</t>
+  </si>
+  <si>
+    <t>Last Verified</t>
   </si>
 </sst>
 </file>
@@ -719,407 +749,600 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C023A292-D7D7-42AA-A66D-EAC889642A87}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="146.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>93</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>96</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data values to requirements_traceability.xlsx
</commit_message>
<xml_diff>
--- a/Evidence/REQM/requirements_traceability.xlsx
+++ b/Evidence/REQM/requirements_traceability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raygu\Downloads\CO3095-Group-16-Music-Player-Application\Evidence\REQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E2C706-65C5-49D8-834B-2D2BD68F6082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A5C9D7-3604-43B1-BEBB-8A37EACE49FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{69E9F38F-E908-4412-9BBE-056D5BFD6B03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="158">
   <si>
     <t>Story ID</t>
   </si>
@@ -360,6 +360,156 @@
   </si>
   <si>
     <t>Last Verified</t>
+  </si>
+  <si>
+    <t>Should</t>
+  </si>
+  <si>
+    <t>play starts/resumes; pause toggles; stop halts &amp; resets; errors handled; state reflected in UI</t>
+  </si>
+  <si>
+    <t>next advances; prev goes back; wrap behavior; single/empty list handling</t>
+  </si>
+  <si>
+    <t>shows title/artist/duration; updates on change; fallback to filename; formatting</t>
+  </si>
+  <si>
+    <t>displays elapsed/total; updates each second; paused stops increment; unknown duration handled</t>
+  </si>
+  <si>
+    <t>text bar matches position; parse mm:ss or seconds; clamp to range; state preserved</t>
+  </si>
+  <si>
+    <t>maps keys; works when UI focused; conflicts handled; repeat-safe</t>
+  </si>
+  <si>
+    <t>ff adds 5s; rw subtracts 5s; clamps; works in paused/playing</t>
+  </si>
+  <si>
+    <t>toggle mute; remember previous volume; set volume while muted updates stored value</t>
+  </si>
+  <si>
+    <t>current track prefixed icon; updates on state changes; accurate index mapping</t>
+  </si>
+  <si>
+    <t>help lists commands &amp; descriptions; help &lt;cmd&gt; shows detail; unknown suggests help</t>
+  </si>
+  <si>
+    <t>separate playback thread/task; CLI non-blocking; graceful shutdown; resource cleanup</t>
+  </si>
+  <si>
+    <t>create playlist; rename existing; delete by name/id; errors for duplicates/not found</t>
+  </si>
+  <si>
+    <t>add by id/path; remove by index/id; reorder by move/swap; persistence</t>
+  </si>
+  <si>
+    <t>case-insensitive search; partial matches; multiple fields; empty result handled</t>
+  </si>
+  <si>
+    <t>tabular layout; columns aligned; pagination if needed; null-safe values</t>
+  </si>
+  <si>
+    <t>list with name &amp; count; select by name/number; errors for invalid</t>
+  </si>
+  <si>
+    <t>show numbered tracks with durations; handles empty; updates on changes</t>
+  </si>
+  <si>
+    <t>add by search result/id; confirm existence; prevent duplicates (or allow as option)</t>
+  </si>
+  <si>
+    <t>success messages include playlist &amp; song; failures include reason; no silent errors</t>
+  </si>
+  <si>
+    <t>scan path recursively; supported extensions only; update library; handle duplicates</t>
+  </si>
+  <si>
+    <t>shows track count and hh:mm:ss; recalculates on change; accurate sum</t>
+  </si>
+  <si>
+    <t>merge A+B; optional remove duplicates; stable order; returns new playlist</t>
+  </si>
+  <si>
+    <t>deep copy retains order; new name required; independent edits</t>
+  </si>
+  <si>
+    <t>toggle shuffle; deterministic with seed; persists state; respects queue</t>
+  </si>
+  <si>
+    <t>loop single track; loop playlist; off state; interactions with next/prev</t>
+  </si>
+  <si>
+    <t>show current queue order; show history list; empty states handled</t>
+  </si>
+  <si>
+    <t>enqueue by id; remove by position/id; no duplicates optional; immediate effect</t>
+  </si>
+  <si>
+    <t>place song at position 1 in queue; respects currently playing; id validation</t>
+  </si>
+  <si>
+    <t>one command clears queue; playback unaffected until next track; confirm message</t>
+  </si>
+  <si>
+    <t>list all liked tracks; sort by date liked or title; empty state handled</t>
+  </si>
+  <si>
+    <t>sort by chosen key; stable sort; reversible; persists order</t>
+  </si>
+  <si>
+    <t>track play counts; list top N; ties deterministic</t>
+  </si>
+  <si>
+    <t>set timer minutes; cancels/overrides; stops playback on expiry; persistence optional</t>
+  </si>
+  <si>
+    <t>persist on exit; load on start; defaults if file missing; error-tolerant</t>
+  </si>
+  <si>
+    <t>define schedules; next-run calculation; execute play at time; overlap handling</t>
+  </si>
+  <si>
+    <t>checkpoint periodically; restore on start; file corruption safe</t>
+  </si>
+  <si>
+    <t>create tags; assign to songs; filter query (AND/OR/basic); persist</t>
+  </si>
+  <si>
+    <t>list by added timestamp; configurable window; empty state handled</t>
+  </si>
+  <si>
+    <t>create/switch profiles; isolated settings/library/playlists; default profile</t>
+  </si>
+  <si>
+    <t>accumulate per track/artist; total listening time; render stats view</t>
+  </si>
+  <si>
+    <t>export fields index/title/artist/duration/path; write CSV; handle IO errors</t>
+  </si>
+  <si>
+    <t>accepts numeric input; clamps 0-100; errors for invalid; immediate effect</t>
+  </si>
+  <si>
+    <t>set rating 1-10; filter by rating; auto playlists per rating</t>
+  </si>
+  <si>
+    <t>edit fields; validation; data persists</t>
+  </si>
+  <si>
+    <t>add/remove changed files; robustness to rapid changes</t>
+  </si>
+  <si>
+    <t>import local/external; skip unsupported; duplicate; progress reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle like; persist per track; </t>
+  </si>
+  <si>
+    <t>accept 0.5-2.0; clamp; persists; affects playback timing</t>
+  </si>
+  <si>
+    <t>Backlog</t>
   </si>
 </sst>
 </file>
@@ -751,15 +901,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C023A292-D7D7-42AA-A66D-EAC889642A87}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="146.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="88.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
@@ -818,6 +969,12 @@
       <c r="D2" t="s">
         <v>100</v>
       </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -832,6 +989,12 @@
       <c r="D3" t="s">
         <v>100</v>
       </c>
+      <c r="E3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -846,6 +1009,12 @@
       <c r="D4" t="s">
         <v>100</v>
       </c>
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -860,6 +1029,12 @@
       <c r="D5" t="s">
         <v>100</v>
       </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -871,6 +1046,15 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -882,6 +1066,15 @@
       <c r="C7">
         <v>1</v>
       </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -893,6 +1086,15 @@
       <c r="C8">
         <v>1</v>
       </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -904,6 +1106,15 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -915,6 +1126,15 @@
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -926,6 +1146,15 @@
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -937,6 +1166,15 @@
       <c r="C12">
         <v>1</v>
       </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -948,6 +1186,15 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -959,6 +1206,15 @@
       <c r="C14">
         <v>2</v>
       </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -970,6 +1226,15 @@
       <c r="C15">
         <v>2</v>
       </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -981,8 +1246,17 @@
       <c r="C16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -992,8 +1266,17 @@
       <c r="C17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1003,8 +1286,17 @@
       <c r="C18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1014,8 +1306,17 @@
       <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1025,8 +1326,17 @@
       <c r="C20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1036,8 +1346,17 @@
       <c r="C21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1047,8 +1366,17 @@
       <c r="C22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1058,8 +1386,17 @@
       <c r="C23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1069,8 +1406,17 @@
       <c r="C24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>130</v>
+      </c>
+      <c r="I24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -1080,8 +1426,17 @@
       <c r="C25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1091,8 +1446,17 @@
       <c r="C26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>132</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -1102,8 +1466,17 @@
       <c r="C27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1113,8 +1486,17 @@
       <c r="C28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" t="s">
+        <v>134</v>
+      </c>
+      <c r="I28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -1124,8 +1506,17 @@
       <c r="C29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+      <c r="I29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -1135,8 +1526,17 @@
       <c r="C30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+      <c r="I30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1146,8 +1546,17 @@
       <c r="C31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
+        <v>137</v>
+      </c>
+      <c r="I31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -1157,8 +1566,17 @@
       <c r="C32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>156</v>
+      </c>
+      <c r="I32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -1168,8 +1586,17 @@
       <c r="C33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" t="s">
+        <v>155</v>
+      </c>
+      <c r="I33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1179,8 +1606,17 @@
       <c r="C34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" t="s">
+        <v>138</v>
+      </c>
+      <c r="I34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -1190,8 +1626,17 @@
       <c r="C35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
+      <c r="I35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -1201,8 +1646,17 @@
       <c r="C36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" t="s">
+        <v>140</v>
+      </c>
+      <c r="I36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -1212,8 +1666,17 @@
       <c r="C37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>141</v>
+      </c>
+      <c r="I37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -1223,8 +1686,17 @@
       <c r="C38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" t="s">
+        <v>142</v>
+      </c>
+      <c r="I38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -1234,8 +1706,17 @@
       <c r="C39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -1245,8 +1726,17 @@
       <c r="C40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" t="s">
+        <v>144</v>
+      </c>
+      <c r="I40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -1256,8 +1746,17 @@
       <c r="C41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" t="s">
+        <v>154</v>
+      </c>
+      <c r="I41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -1267,8 +1766,17 @@
       <c r="C42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -1278,8 +1786,17 @@
       <c r="C43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" t="s">
+        <v>146</v>
+      </c>
+      <c r="I43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -1289,8 +1806,17 @@
       <c r="C44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" t="s">
+        <v>147</v>
+      </c>
+      <c r="I44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -1300,8 +1826,17 @@
       <c r="C45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -1311,8 +1846,17 @@
       <c r="C46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -1322,8 +1866,17 @@
       <c r="C47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -1333,8 +1886,17 @@
       <c r="C48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" t="s">
+        <v>152</v>
+      </c>
+      <c r="I48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -1343,6 +1905,15 @@
       </c>
       <c r="C49">
         <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" t="s">
+        <v>151</v>
+      </c>
+      <c r="I49" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>